<commit_message>
Basic generic dot renderer.
</commit_message>
<xml_diff>
--- a/hotrod/testdata/databases/postgresql-9.4/plan/design.xlsx
+++ b/hotrod/testdata/databases/postgresql-9.4/plan/design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="39">
   <si>
     <t xml:space="preserve">Estimate</t>
   </si>
@@ -294,6 +294,30 @@
   </si>
   <si>
     <t xml:space="preserve">est. 78 rows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Metrics</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">137</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF999999"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ms</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -648,7 +672,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -657,10 +681,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -733,10 +753,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -839,6 +855,22 @@
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -918,65 +950,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N47"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L53" activeCellId="0" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.13775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.27551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.27551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.0867346938776"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="12.0867346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="0"/>
+      <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0"/>
       <c r="G3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="0"/>
       <c r="G4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F5" s="5"/>
+      <c r="D5" s="0"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="0"/>
+      <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -990,10 +1030,11 @@
       <c r="C8" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="0"/>
       <c r="G8" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1004,10 +1045,11 @@
       <c r="C9" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="D9" s="0"/>
       <c r="G9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1018,6 +1060,7 @@
       <c r="C10" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="D10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
@@ -1026,339 +1069,477 @@
       <c r="C11" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="D11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="0"/>
+      <c r="F12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="D13" s="0"/>
       <c r="G13" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D14" s="0"/>
       <c r="G14" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="7" t="s">
+      <c r="D15" s="0"/>
+      <c r="G15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="11" t="n">
+      <c r="K19" s="3"/>
+      <c r="L19" s="10" t="n">
         <v>137</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="M19" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="13" t="s">
+      <c r="D20" s="0"/>
+      <c r="F20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="1"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="15" t="s">
+      <c r="L20" s="12"/>
+      <c r="M20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="N20" s="15"/>
+      <c r="N20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="16"/>
-      <c r="G21" s="17" t="s">
+      <c r="D21" s="0"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16" t="s">
         <v>23</v>
       </c>
       <c r="J21" s="1"/>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="17" t="s">
+      <c r="M21" s="17"/>
+      <c r="N21" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="5"/>
-      <c r="F22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="5"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="21"/>
+      <c r="D22" s="4"/>
+      <c r="F22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="4"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="19"/>
+      <c r="D23" s="0"/>
+      <c r="F23" s="18"/>
       <c r="J23" s="1"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="21"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="8" t="s">
+      <c r="I24" s="5"/>
+      <c r="J24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="23" t="s">
+      <c r="K24" s="3"/>
+      <c r="L24" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="M24" s="24"/>
-      <c r="N24" s="10" t="s">
+      <c r="M24" s="22"/>
+      <c r="N24" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="25" t="s">
+      <c r="D25" s="0"/>
+      <c r="F25" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="14" t="s">
+      <c r="L25" s="23"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="27" t="s">
+      <c r="D26" s="0"/>
+      <c r="F26" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="16" t="s">
         <v>23</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="L26" s="27" t="s">
+      <c r="L26" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="28"/>
-      <c r="N26" s="17" t="s">
+      <c r="M26" s="26"/>
+      <c r="N26" s="16" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="19"/>
+      <c r="D27" s="0"/>
+      <c r="F27" s="18"/>
       <c r="J27" s="1"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="21"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="19"/>
+      <c r="D28" s="0"/>
+      <c r="F28" s="18"/>
       <c r="J28" s="1"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="21"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="22" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="J29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K29" s="4"/>
-      <c r="L29" s="29" t="s">
+      <c r="K29" s="3"/>
+      <c r="L29" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="24"/>
-      <c r="N29" s="10" t="s">
+      <c r="M29" s="22"/>
+      <c r="N29" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="25" t="s">
+      <c r="D30" s="0"/>
+      <c r="F30" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>22</v>
       </c>
       <c r="J30" s="1"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="14" t="s">
+      <c r="L30" s="23"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="25" t="s">
+      <c r="D31" s="0"/>
+      <c r="F31" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="28" t="s">
         <v>23</v>
       </c>
       <c r="J31" s="1"/>
-      <c r="L31" s="25" t="s">
+      <c r="L31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="26"/>
-      <c r="N31" s="30" t="s">
+      <c r="M31" s="24"/>
+      <c r="N31" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E32" s="31"/>
-      <c r="F32" s="32" t="s">
+      <c r="D32" s="0"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="32"/>
+      <c r="G32" s="30"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="32" t="s">
+      <c r="K32" s="29"/>
+      <c r="L32" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J35" s="8" t="s">
+      <c r="D35" s="0"/>
+      <c r="J35" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L35" s="11" t="s">
+      <c r="L35" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M35" s="33" t="s">
+      <c r="M35" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="N35" s="34"/>
+      <c r="N35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L36" s="35" t="s">
+      <c r="D36" s="0"/>
+      <c r="L36" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="M36" s="36"/>
-      <c r="N36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="38" t="s">
+      <c r="G37" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="L37" s="39" t="s">
+      <c r="L37" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="M37" s="40" t="s">
+      <c r="M37" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="N37" s="41"/>
+      <c r="N37" s="39"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G38" s="38" t="s">
+      <c r="G38" s="36" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J39" s="8" t="s">
+      <c r="J39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L39" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="M39" s="33" t="s">
+      <c r="M39" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="M40" s="36"/>
+      <c r="M40" s="34"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L41" s="39" t="s">
+      <c r="L41" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="M41" s="40" t="s">
+      <c r="M41" s="38" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L42" s="42"/>
-      <c r="M42" s="43"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="41"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J44" s="8" t="s">
+      <c r="J44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L44" s="29" t="s">
+      <c r="L44" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="M44" s="33" t="s">
+      <c r="M44" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L45" s="35" t="s">
+      <c r="L45" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="M45" s="36"/>
+      <c r="M45" s="34"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L46" s="44" t="s">
+      <c r="L46" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="M46" s="45" t="s">
+      <c r="M46" s="43" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L47" s="46" t="s">
+      <c r="L47" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="M47" s="47" t="s">
+      <c r="M47" s="45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L51" s="46"/>
+      <c r="M51" s="47"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J52" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="M52" s="49"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L53" s="37"/>
+      <c r="M53" s="38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L55" s="10" t="n">
+        <v>137</v>
+      </c>
+      <c r="M55" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L56" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M56" s="34"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L57" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" s="38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L59" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M59" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L60" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M60" s="34"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L61" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="M61" s="38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L62" s="40"/>
+      <c r="M62" s="41"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J64" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L64" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="M64" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L65" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M65" s="34"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L66" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="M66" s="43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L67" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M67" s="45" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>